<commit_message>
new gnn figs and tables
</commit_message>
<xml_diff>
--- a/Output/Modelling/Graph Neural Network/Tables/Inductive_model_comparison_df.xlsx
+++ b/Output/Modelling/Graph Neural Network/Tables/Inductive_model_comparison_df.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5049751243781094</v>
+        <v>0.6169154228855721</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5373134328358209</v>
+        <v>0.6467661691542289</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
ggn lte 1 from actual
</commit_message>
<xml_diff>
--- a/Output/Modelling/Graph Neural Network/Tables/Inductive_model_comparison_df.xlsx
+++ b/Output/Modelling/Graph Neural Network/Tables/Inductive_model_comparison_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Accuracy</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Share $\le$ 1 Rating From Actual</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -454,6 +459,11 @@
       <c r="B2" t="n">
         <v>0.3134328358208955</v>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.7687</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -464,6 +474,11 @@
       <c r="B3" t="n">
         <v>0.6169154228855721</v>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.9204</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -474,6 +489,11 @@
       <c r="B4" t="n">
         <v>0.6467661691542289</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.9378</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -484,6 +504,7 @@
       <c r="B5" t="n">
         <v>0.2985074626865671</v>
       </c>
+      <c r="C5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>